<commit_message>
finished draft of intro
</commit_message>
<xml_diff>
--- a/data/literature_flux_summary.xlsx
+++ b/data/literature_flux_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sara/Code/Research/2022_Young_Hogg_Comparison/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ECB68A-916D-0A4B-97D9-7154D211C119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007DAB6C-052B-BE41-9CF2-DFD0E0DC7AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35800" yWindow="3580" windowWidth="28040" windowHeight="16940" xr2:uid="{3646D1CD-9235-2F48-8DF5-1EB92F23C899}"/>
   </bookViews>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10FC323-FC3C-E74D-901A-1016D56C1C31}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>